<commit_message>
Improve phone extraction regex and evaluation reporting
Enhanced the phone number regex in rule.py to better match various Vietnamese phone formats. Updated test.py to track and report false positive/negative indices and provide detailed exact match error information in the evaluation report for improved debugging and analysis.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hcmuteduvn-my.sharepoint.com/personal/tan_vonhatcse_hcmut_edu_vn/Documents/Tài liệu/HCMUT/URA/Project SYT/NER/extract-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_3761651F6BFA0BBDC9717A66E34CF4F0C0C0B2E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BC0D42E-34DA-4B8E-B6A8-E5DFEEAEFA52}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="11_3761651F6BFA0BBDC9717A66E34CF4F0C0C0B2E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FEED3AF-3C7B-4FC0-85E2-2C5EFB75E553}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1449,7 +1449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1464,6 +1464,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1685,18 +1690,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
+      <selection activeCell="B223" sqref="B223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="3" width="90.77734375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="90.796875" style="7" customWidth="1"/>
+    <col min="2" max="3" width="90.796875" style="3" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:26" ht="18" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1706,8 +1712,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="198" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:26" ht="180" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1717,8 +1723,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="360" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:26" ht="342" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1728,8 +1734,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="234" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:26" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1739,8 +1745,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="216" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:26" ht="198" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1750,8 +1756,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="180" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:26" ht="180" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1761,8 +1767,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="198" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:26" ht="180" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1772,8 +1778,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="288" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:26" ht="270" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1783,8 +1789,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="360" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:26" ht="360" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1794,8 +1800,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="234" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:26" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1805,8 +1811,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="234" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:26" ht="216" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1816,8 +1822,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="54" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:26" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1827,8 +1833,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="306" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:26" ht="306" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1838,8 +1844,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="288" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:26" ht="270" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1872,8 +1878,8 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="72" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:26" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1883,8 +1889,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="252" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:26" ht="234" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1894,8 +1900,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:26" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1905,8 +1911,8 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="360" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:26" ht="324" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1916,8 +1922,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="288" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:26" ht="270" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1927,8 +1933,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="18" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:26" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1938,8 +1944,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1949,8 +1955,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -1983,8 +1989,8 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1994,8 +2000,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -2005,8 +2011,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2016,8 +2022,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2027,8 +2033,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2038,8 +2044,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2049,8 +2055,8 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2060,8 +2066,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2071,8 +2077,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2082,8 +2088,8 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2093,8 +2099,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2104,8 +2110,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2115,8 +2121,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2126,8 +2132,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2137,8 +2143,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2148,8 +2154,8 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2159,8 +2165,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2170,8 +2176,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="4" t="s">
@@ -2204,8 +2210,8 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2215,8 +2221,8 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2226,8 +2232,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2237,8 +2243,8 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2248,7 +2254,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
         <v>87</v>
       </c>
@@ -2259,8 +2265,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2270,8 +2276,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -2281,8 +2287,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -2292,8 +2298,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -2303,8 +2309,8 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2314,8 +2320,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -2325,8 +2331,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -2336,8 +2342,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -2347,8 +2353,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -2358,8 +2364,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -2369,8 +2375,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" s="7" t="s">
         <v>110</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -2380,8 +2386,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -2391,8 +2397,8 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -2402,8 +2408,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="3" t="s">
+    <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -2413,8 +2419,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="8" t="s">
         <v>116</v>
       </c>
       <c r="B60" s="4" t="s">
@@ -2447,8 +2453,8 @@
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="3" t="s">
+    <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -2458,8 +2464,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
+    <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -2469,8 +2475,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="7" t="s">
         <v>124</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -2480,8 +2486,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="7" t="s">
         <v>126</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -2491,8 +2497,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="3" t="s">
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="7" t="s">
         <v>128</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -2502,8 +2508,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -2513,8 +2519,8 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="7" t="s">
         <v>132</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -2524,8 +2530,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -2535,8 +2541,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="s">
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="7" t="s">
         <v>135</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -2546,8 +2552,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="3" t="s">
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="7" t="s">
         <v>136</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -2557,8 +2563,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="s">
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="7" t="s">
         <v>139</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -2568,8 +2574,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="3" t="s">
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -2579,8 +2585,8 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="3" t="s">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -2590,8 +2596,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="3" t="s">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -2601,8 +2607,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="3" t="s">
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -2612,8 +2618,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -2623,8 +2629,8 @@
         <v>151</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="7" t="s">
         <v>152</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -2634,8 +2640,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="3" t="s">
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -2645,8 +2651,8 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="3" t="s">
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="7" t="s">
         <v>156</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -2656,8 +2662,8 @@
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="3" t="s">
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="7" t="s">
         <v>159</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -2667,8 +2673,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="3" t="s">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="7" t="s">
         <v>162</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -2678,8 +2684,8 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="7" t="s">
         <v>164</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -2689,8 +2695,8 @@
         <v>166</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="3" t="s">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="7" t="s">
         <v>167</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -2700,8 +2706,8 @@
         <v>169</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="3" t="s">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="7" t="s">
         <v>170</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -2711,8 +2717,8 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="3" t="s">
+    <row r="85" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="7" t="s">
         <v>172</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -2722,8 +2728,8 @@
         <v>174</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="3" t="s">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="7" t="s">
         <v>175</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -2733,8 +2739,8 @@
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="3" t="s">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" s="7" t="s">
         <v>176</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -2744,8 +2750,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" s="7" t="s">
         <v>177</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -2755,8 +2761,8 @@
         <v>179</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="3" t="s">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" s="7" t="s">
         <v>180</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -2766,8 +2772,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="3" t="s">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="7" t="s">
         <v>181</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -2777,8 +2783,8 @@
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="3" t="s">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="7" t="s">
         <v>182</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -2788,8 +2794,8 @@
         <v>184</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="3" t="s">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="7" t="s">
         <v>185</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -2799,8 +2805,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="7" t="s">
         <v>186</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -2810,8 +2816,8 @@
         <v>188</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="3" t="s">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="7" t="s">
         <v>189</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -2821,8 +2827,8 @@
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="3" t="s">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="7" t="s">
         <v>192</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -2832,8 +2838,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="3" t="s">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="7" t="s">
         <v>194</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -2843,8 +2849,8 @@
         <v>195</v>
       </c>
     </row>
-    <row r="97" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="3" t="s">
+    <row r="97" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="7" t="s">
         <v>196</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -2854,8 +2860,8 @@
         <v>197</v>
       </c>
     </row>
-    <row r="98" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="3" t="s">
+    <row r="98" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="7" t="s">
         <v>198</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -2865,8 +2871,8 @@
         <v>198</v>
       </c>
     </row>
-    <row r="99" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="3" t="s">
+    <row r="99" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="7" t="s">
         <v>200</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -2876,8 +2882,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="100" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
+    <row r="100" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="7" t="s">
         <v>203</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -2887,8 +2893,8 @@
         <v>203</v>
       </c>
     </row>
-    <row r="101" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="4" t="s">
+    <row r="101" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="8" t="s">
         <v>204</v>
       </c>
       <c r="B101" s="4" t="s">
@@ -2921,8 +2927,8 @@
       <c r="Y101" s="1"/>
       <c r="Z101" s="1"/>
     </row>
-    <row r="102" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="4" t="s">
+    <row r="102" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="8" t="s">
         <v>207</v>
       </c>
       <c r="B102" s="4" t="s">
@@ -2955,8 +2961,8 @@
       <c r="Y102" s="1"/>
       <c r="Z102" s="1"/>
     </row>
-    <row r="103" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="s">
+    <row r="103" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="7" t="s">
         <v>209</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -2966,8 +2972,8 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="3" t="s">
+    <row r="104" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="7" t="s">
         <v>210</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -2977,8 +2983,8 @@
         <v>210</v>
       </c>
     </row>
-    <row r="105" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="3" t="s">
+    <row r="105" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="7" t="s">
         <v>211</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -2988,8 +2994,8 @@
         <v>213</v>
       </c>
     </row>
-    <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="3" t="s">
+    <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="7" t="s">
         <v>214</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -2999,8 +3005,8 @@
         <v>215</v>
       </c>
     </row>
-    <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="3" t="s">
+    <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="7" t="s">
         <v>216</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -3010,8 +3016,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="108" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="3" t="s">
+    <row r="108" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="7" t="s">
         <v>219</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -3021,8 +3027,8 @@
         <v>219</v>
       </c>
     </row>
-    <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="3" t="s">
+    <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="7" t="s">
         <v>220</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -3032,8 +3038,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="3" t="s">
+    <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="7" t="s">
         <v>222</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -3043,8 +3049,8 @@
         <v>222</v>
       </c>
     </row>
-    <row r="111" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="3" t="s">
+    <row r="111" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="7" t="s">
         <v>224</v>
       </c>
       <c r="B111" s="3" t="s">
@@ -3054,8 +3060,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="3" t="s">
+    <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="7" t="s">
         <v>225</v>
       </c>
       <c r="B112" s="3" t="s">
@@ -3065,8 +3071,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="3" t="s">
+    <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" s="7" t="s">
         <v>227</v>
       </c>
       <c r="B113" s="3" t="s">
@@ -3076,8 +3082,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="3" t="s">
+    <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" s="7" t="s">
         <v>229</v>
       </c>
       <c r="B114" s="3" t="s">
@@ -3087,8 +3093,8 @@
         <v>231</v>
       </c>
     </row>
-    <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="3" t="s">
+    <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" s="7" t="s">
         <v>232</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -3098,8 +3104,8 @@
         <v>234</v>
       </c>
     </row>
-    <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="4" t="s">
+    <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116" s="8" t="s">
         <v>235</v>
       </c>
       <c r="B116" s="4" t="s">
@@ -3132,8 +3138,8 @@
       <c r="Y116" s="1"/>
       <c r="Z116" s="1"/>
     </row>
-    <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="s">
+    <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" s="7" t="s">
         <v>237</v>
       </c>
       <c r="B117" s="3" t="s">
@@ -3143,8 +3149,8 @@
         <v>239</v>
       </c>
     </row>
-    <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="3" t="s">
+    <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118" s="7" t="s">
         <v>240</v>
       </c>
       <c r="B118" s="3" t="s">
@@ -3154,8 +3160,8 @@
         <v>242</v>
       </c>
     </row>
-    <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="3" t="s">
+    <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" s="7" t="s">
         <v>243</v>
       </c>
       <c r="B119" s="3" t="s">
@@ -3165,8 +3171,8 @@
         <v>244</v>
       </c>
     </row>
-    <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="3" t="s">
+    <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" s="7" t="s">
         <v>245</v>
       </c>
       <c r="B120" s="3" t="s">
@@ -3176,8 +3182,8 @@
         <v>247</v>
       </c>
     </row>
-    <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="3" t="s">
+    <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" s="7" t="s">
         <v>248</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -3187,8 +3193,8 @@
         <v>249</v>
       </c>
     </row>
-    <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="3" t="s">
+    <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="7" t="s">
         <v>250</v>
       </c>
       <c r="B122" s="3" t="s">
@@ -3198,8 +3204,8 @@
         <v>252</v>
       </c>
     </row>
-    <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="3" t="s">
+    <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="7" t="s">
         <v>253</v>
       </c>
       <c r="B123" s="3" t="s">
@@ -3209,8 +3215,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="3" t="s">
+    <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="7" t="s">
         <v>254</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -3220,8 +3226,8 @@
         <v>256</v>
       </c>
     </row>
-    <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="3" t="s">
+    <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="7" t="s">
         <v>257</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -3231,8 +3237,8 @@
         <v>259</v>
       </c>
     </row>
-    <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="3" t="s">
+    <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="7" t="s">
         <v>260</v>
       </c>
       <c r="B126" s="3" t="s">
@@ -3242,8 +3248,8 @@
         <v>261</v>
       </c>
     </row>
-    <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="3" t="s">
+    <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="7" t="s">
         <v>262</v>
       </c>
       <c r="B127" s="3" t="s">
@@ -3253,8 +3259,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="3" t="s">
+    <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="7" t="s">
         <v>263</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -3264,8 +3270,8 @@
         <v>263</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="s">
+    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="7" t="s">
         <v>264</v>
       </c>
       <c r="B129" s="3" t="s">
@@ -3275,8 +3281,8 @@
         <v>264</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="3" t="s">
+    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="7" t="s">
         <v>265</v>
       </c>
       <c r="B130" s="3" t="s">
@@ -3286,8 +3292,8 @@
         <v>265</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="3" t="s">
+    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="7" t="s">
         <v>266</v>
       </c>
       <c r="B131" s="3" t="s">
@@ -3297,8 +3303,8 @@
         <v>266</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="3" t="s">
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="7" t="s">
         <v>267</v>
       </c>
       <c r="B132" s="3" t="s">
@@ -3308,8 +3314,8 @@
         <v>269</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="3" t="s">
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="7" t="s">
         <v>270</v>
       </c>
       <c r="B133" s="3" t="s">
@@ -3319,8 +3325,8 @@
         <v>272</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="3" t="s">
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="7" t="s">
         <v>273</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -3330,8 +3336,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="3" t="s">
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="7" t="s">
         <v>276</v>
       </c>
       <c r="B135" s="3" t="s">
@@ -3341,8 +3347,8 @@
         <v>278</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="3" t="s">
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="7" t="s">
         <v>279</v>
       </c>
       <c r="B136" s="3" t="s">
@@ -3352,8 +3358,8 @@
         <v>280</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="3" t="s">
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="7" t="s">
         <v>281</v>
       </c>
       <c r="B137" s="3" t="s">
@@ -3363,8 +3369,8 @@
         <v>281</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="3" t="s">
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="7" t="s">
         <v>282</v>
       </c>
       <c r="B138" s="3" t="s">
@@ -3374,8 +3380,8 @@
         <v>283</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="3" t="s">
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="7" t="s">
         <v>284</v>
       </c>
       <c r="B139" s="3" t="s">
@@ -3385,8 +3391,8 @@
         <v>284</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A140" s="3" t="s">
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="7" t="s">
         <v>285</v>
       </c>
       <c r="B140" s="3" t="s">
@@ -3396,8 +3402,8 @@
         <v>287</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A141" s="3" t="s">
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="7" t="s">
         <v>288</v>
       </c>
       <c r="B141" s="3" t="s">
@@ -3407,8 +3413,8 @@
         <v>288</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A142" s="3" t="s">
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="7" t="s">
         <v>290</v>
       </c>
       <c r="B142" s="3" t="s">
@@ -3418,8 +3424,8 @@
         <v>290</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A143" s="3" t="s">
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="7" t="s">
         <v>291</v>
       </c>
       <c r="B143" s="3" t="s">
@@ -3429,8 +3435,8 @@
         <v>292</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A144" s="3" t="s">
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="7" t="s">
         <v>293</v>
       </c>
       <c r="B144" s="3" t="s">
@@ -3440,8 +3446,8 @@
         <v>293</v>
       </c>
     </row>
-    <row r="145" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A145" s="3" t="s">
+    <row r="145" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="7" t="s">
         <v>294</v>
       </c>
       <c r="B145" s="3" t="s">
@@ -3451,8 +3457,8 @@
         <v>296</v>
       </c>
     </row>
-    <row r="146" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A146" s="3" t="s">
+    <row r="146" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" s="7" t="s">
         <v>297</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -3462,8 +3468,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A147" s="3" t="s">
+    <row r="147" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="7" t="s">
         <v>300</v>
       </c>
       <c r="B147" s="3" t="s">
@@ -3473,8 +3479,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="148" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A148" s="3" t="s">
+    <row r="148" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" s="7" t="s">
         <v>302</v>
       </c>
       <c r="B148" s="3" t="s">
@@ -3484,8 +3490,8 @@
         <v>303</v>
       </c>
     </row>
-    <row r="149" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A149" s="3" t="s">
+    <row r="149" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" s="7" t="s">
         <v>304</v>
       </c>
       <c r="B149" s="3" t="s">
@@ -3495,8 +3501,8 @@
         <v>305</v>
       </c>
     </row>
-    <row r="150" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A150" s="3" t="s">
+    <row r="150" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" s="7" t="s">
         <v>306</v>
       </c>
       <c r="B150" s="3" t="s">
@@ -3506,8 +3512,8 @@
         <v>307</v>
       </c>
     </row>
-    <row r="151" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="4" t="s">
+    <row r="151" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" s="8" t="s">
         <v>308</v>
       </c>
       <c r="B151" s="4" t="s">
@@ -3540,8 +3546,8 @@
       <c r="Y151" s="1"/>
       <c r="Z151" s="1"/>
     </row>
-    <row r="152" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A152" s="3" t="s">
+    <row r="152" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" s="7" t="s">
         <v>311</v>
       </c>
       <c r="B152" s="3" t="s">
@@ -3551,8 +3557,8 @@
         <v>313</v>
       </c>
     </row>
-    <row r="153" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A153" s="4" t="s">
+    <row r="153" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153" s="8" t="s">
         <v>314</v>
       </c>
       <c r="B153" s="4" t="s">
@@ -3585,8 +3591,8 @@
       <c r="Y153" s="1"/>
       <c r="Z153" s="1"/>
     </row>
-    <row r="154" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="3" t="s">
+    <row r="154" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="7" t="s">
         <v>316</v>
       </c>
       <c r="B154" s="3" t="s">
@@ -3596,8 +3602,8 @@
         <v>317</v>
       </c>
     </row>
-    <row r="155" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="3" t="s">
+    <row r="155" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" s="7" t="s">
         <v>318</v>
       </c>
       <c r="B155" s="3" t="s">
@@ -3607,8 +3613,8 @@
         <v>318</v>
       </c>
     </row>
-    <row r="156" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A156" s="3" t="s">
+    <row r="156" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" s="7" t="s">
         <v>319</v>
       </c>
       <c r="B156" s="3" t="s">
@@ -3618,8 +3624,8 @@
         <v>319</v>
       </c>
     </row>
-    <row r="157" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A157" s="3" t="s">
+    <row r="157" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" s="7" t="s">
         <v>320</v>
       </c>
       <c r="B157" s="3" t="s">
@@ -3629,8 +3635,8 @@
         <v>320</v>
       </c>
     </row>
-    <row r="158" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="3" t="s">
+    <row r="158" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" s="7" t="s">
         <v>321</v>
       </c>
       <c r="B158" s="3" t="s">
@@ -3640,8 +3646,8 @@
         <v>323</v>
       </c>
     </row>
-    <row r="159" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A159" s="3" t="s">
+    <row r="159" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" s="7" t="s">
         <v>324</v>
       </c>
       <c r="B159" s="3" t="s">
@@ -3651,8 +3657,8 @@
         <v>325</v>
       </c>
     </row>
-    <row r="160" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="3" t="s">
+    <row r="160" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" s="7" t="s">
         <v>326</v>
       </c>
       <c r="B160" s="3" t="s">
@@ -3662,8 +3668,8 @@
         <v>326</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A161" s="3" t="s">
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" s="7" t="s">
         <v>327</v>
       </c>
       <c r="B161" s="3" t="s">
@@ -3673,8 +3679,8 @@
         <v>328</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A162" s="3" t="s">
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="7" t="s">
         <v>329</v>
       </c>
       <c r="B162" s="3" t="s">
@@ -3684,8 +3690,8 @@
         <v>331</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="3" t="s">
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="7" t="s">
         <v>332</v>
       </c>
       <c r="B163" s="3" t="s">
@@ -3695,8 +3701,8 @@
         <v>332</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="3" t="s">
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" s="7" t="s">
         <v>334</v>
       </c>
       <c r="B164" s="3" t="s">
@@ -3706,8 +3712,8 @@
         <v>336</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="3" t="s">
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" s="7" t="s">
         <v>337</v>
       </c>
       <c r="B165" s="3" t="s">
@@ -3717,8 +3723,8 @@
         <v>339</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A166" s="3" t="s">
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="7" t="s">
         <v>340</v>
       </c>
       <c r="B166" s="3" t="s">
@@ -3728,8 +3734,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A167" s="3" t="s">
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" s="7" t="s">
         <v>341</v>
       </c>
       <c r="B167" s="3" t="s">
@@ -3739,8 +3745,8 @@
         <v>342</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A168" s="3" t="s">
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" s="7" t="s">
         <v>343</v>
       </c>
       <c r="B168" s="3" t="s">
@@ -3750,8 +3756,8 @@
         <v>344</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A169" s="3" t="s">
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" s="7" t="s">
         <v>345</v>
       </c>
       <c r="B169" s="3" t="s">
@@ -3761,8 +3767,8 @@
         <v>345</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A170" s="3" t="s">
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" s="7" t="s">
         <v>346</v>
       </c>
       <c r="B170" s="3" t="s">
@@ -3772,8 +3778,8 @@
         <v>348</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A171" s="3" t="s">
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" s="7" t="s">
         <v>349</v>
       </c>
       <c r="B171" s="3" t="s">
@@ -3783,8 +3789,8 @@
         <v>350</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A172" s="3" t="s">
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" s="7" t="s">
         <v>351</v>
       </c>
       <c r="B172" s="3" t="s">
@@ -3794,8 +3800,8 @@
         <v>353</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A173" s="3" t="s">
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" s="7" t="s">
         <v>354</v>
       </c>
       <c r="B173" s="3" t="s">
@@ -3805,8 +3811,8 @@
         <v>356</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A174" s="3" t="s">
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" s="7" t="s">
         <v>357</v>
       </c>
       <c r="B174" s="3" t="s">
@@ -3816,8 +3822,8 @@
         <v>358</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A175" s="3" t="s">
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" s="7" t="s">
         <v>359</v>
       </c>
       <c r="B175" s="3" t="s">
@@ -3827,8 +3833,8 @@
         <v>361</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A176" s="3" t="s">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" s="7" t="s">
         <v>362</v>
       </c>
       <c r="B176" s="3" t="s">
@@ -3838,8 +3844,8 @@
         <v>364</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A177" s="3" t="s">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" s="7" t="s">
         <v>365</v>
       </c>
       <c r="B177" s="3" t="s">
@@ -3849,8 +3855,8 @@
         <v>366</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A178" s="3" t="s">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" s="7" t="s">
         <v>367</v>
       </c>
       <c r="B178" s="3" t="s">
@@ -3860,8 +3866,8 @@
         <v>369</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A179" s="3" t="s">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" s="7" t="s">
         <v>370</v>
       </c>
       <c r="B179" s="3" t="s">
@@ -3871,8 +3877,8 @@
         <v>371</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A180" s="3" t="s">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" s="7" t="s">
         <v>372</v>
       </c>
       <c r="B180" s="3" t="s">
@@ -3882,8 +3888,8 @@
         <v>373</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A181" s="3" t="s">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" s="7" t="s">
         <v>374</v>
       </c>
       <c r="B181" s="3" t="s">
@@ -3893,8 +3899,8 @@
         <v>374</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A182" s="3" t="s">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" s="7" t="s">
         <v>375</v>
       </c>
       <c r="B182" s="3" t="s">
@@ -3904,8 +3910,8 @@
         <v>377</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A183" s="3" t="s">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" s="7" t="s">
         <v>378</v>
       </c>
       <c r="B183" s="3" t="s">
@@ -3915,8 +3921,8 @@
         <v>378</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A184" s="3" t="s">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" s="7" t="s">
         <v>379</v>
       </c>
       <c r="B184" s="3" t="s">
@@ -3926,8 +3932,8 @@
         <v>379</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A185" s="3" t="s">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" s="7" t="s">
         <v>380</v>
       </c>
       <c r="B185" s="3" t="s">
@@ -3937,8 +3943,8 @@
         <v>380</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A186" s="3" t="s">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" s="7" t="s">
         <v>381</v>
       </c>
       <c r="B186" s="3" t="s">
@@ -3948,8 +3954,8 @@
         <v>381</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A187" s="3" t="s">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" s="7" t="s">
         <v>382</v>
       </c>
       <c r="B187" s="3" t="s">
@@ -3959,8 +3965,8 @@
         <v>383</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="3" t="s">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" s="7" t="s">
         <v>384</v>
       </c>
       <c r="B188" s="3" t="s">
@@ -3970,8 +3976,8 @@
         <v>384</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A189" s="3" t="s">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" s="7" t="s">
         <v>385</v>
       </c>
       <c r="B189" s="3" t="s">
@@ -3981,8 +3987,8 @@
         <v>387</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A190" s="3" t="s">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="7" t="s">
         <v>388</v>
       </c>
       <c r="B190" s="3" t="s">
@@ -3992,8 +3998,8 @@
         <v>388</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A191" s="3" t="s">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191" s="7" t="s">
         <v>390</v>
       </c>
       <c r="B191" s="3" t="s">
@@ -4003,8 +4009,8 @@
         <v>392</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A192" s="3" t="s">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" s="7" t="s">
         <v>393</v>
       </c>
       <c r="B192" s="3" t="s">
@@ -4014,8 +4020,8 @@
         <v>393</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A193" s="3" t="s">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" s="7" t="s">
         <v>394</v>
       </c>
       <c r="B193" s="3" t="s">
@@ -4025,8 +4031,8 @@
         <v>394</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A194" s="3" t="s">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" s="7" t="s">
         <v>395</v>
       </c>
       <c r="B194" s="3" t="s">
@@ -4036,8 +4042,8 @@
         <v>395</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A195" s="3" t="s">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="7" t="s">
         <v>396</v>
       </c>
       <c r="B195" s="3" t="s">
@@ -4047,8 +4053,8 @@
         <v>396</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A196" s="3" t="s">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" s="7" t="s">
         <v>397</v>
       </c>
       <c r="B196" s="3" t="s">
@@ -4058,8 +4064,8 @@
         <v>398</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A197" s="3" t="s">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" s="7" t="s">
         <v>399</v>
       </c>
       <c r="B197" s="3" t="s">
@@ -4069,8 +4075,8 @@
         <v>400</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A198" s="3" t="s">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" s="7" t="s">
         <v>401</v>
       </c>
       <c r="B198" s="3" t="s">
@@ -4080,8 +4086,8 @@
         <v>401</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A199" s="3" t="s">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" s="7" t="s">
         <v>402</v>
       </c>
       <c r="B199" s="3" t="s">
@@ -4091,8 +4097,8 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="3" t="s">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" s="7" t="s">
         <v>403</v>
       </c>
       <c r="B200" s="3" t="s">
@@ -4102,8 +4108,8 @@
         <v>403</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A201" s="3" t="s">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" s="7" t="s">
         <v>404</v>
       </c>
       <c r="B201" s="3" t="s">
@@ -4113,8 +4119,8 @@
         <v>405</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A202" s="3" t="s">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A202" s="7" t="s">
         <v>406</v>
       </c>
       <c r="B202" s="3" t="s">
@@ -4124,8 +4130,8 @@
         <v>407</v>
       </c>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A203" s="3" t="s">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203" s="7" t="s">
         <v>408</v>
       </c>
       <c r="B203" s="3" t="s">
@@ -4135,8 +4141,8 @@
         <v>408</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A204" s="3" t="s">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204" s="7" t="s">
         <v>409</v>
       </c>
       <c r="B204" s="3" t="s">
@@ -4146,8 +4152,8 @@
         <v>410</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A205" s="3" t="s">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A205" s="7" t="s">
         <v>411</v>
       </c>
       <c r="B205" s="3" t="s">
@@ -4157,8 +4163,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A206" s="3" t="s">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A206" s="7" t="s">
         <v>413</v>
       </c>
       <c r="B206" s="3" t="s">
@@ -4168,8 +4174,8 @@
         <v>414</v>
       </c>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A207" s="3" t="s">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207" s="7" t="s">
         <v>415</v>
       </c>
       <c r="B207" s="3" t="s">
@@ -4179,8 +4185,8 @@
         <v>416</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A208" s="3" t="s">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" s="7" t="s">
         <v>417</v>
       </c>
       <c r="B208" s="3" t="s">
@@ -4190,8 +4196,8 @@
         <v>418</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A209" s="3" t="s">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A209" s="7" t="s">
         <v>419</v>
       </c>
       <c r="B209" s="3" t="s">
@@ -4201,8 +4207,8 @@
         <v>420</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A210" s="3" t="s">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210" s="7" t="s">
         <v>421</v>
       </c>
       <c r="B210" s="3" t="s">
@@ -4212,8 +4218,8 @@
         <v>422</v>
       </c>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A211" s="3" t="s">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211" s="7" t="s">
         <v>423</v>
       </c>
       <c r="B211" s="3" t="s">
@@ -4223,8 +4229,8 @@
         <v>423</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A212" s="3" t="s">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A212" s="7" t="s">
         <v>424</v>
       </c>
       <c r="B212" s="3" t="s">
@@ -4234,8 +4240,8 @@
         <v>424</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A213" s="3" t="s">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A213" s="7" t="s">
         <v>425</v>
       </c>
       <c r="B213" s="3" t="s">
@@ -4245,8 +4251,8 @@
         <v>426</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A214" s="3" t="s">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A214" s="7" t="s">
         <v>427</v>
       </c>
       <c r="B214" s="3" t="s">
@@ -4256,8 +4262,8 @@
         <v>427</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A215" s="3" t="s">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A215" s="7" t="s">
         <v>428</v>
       </c>
       <c r="B215" s="3" t="s">
@@ -4267,8 +4273,8 @@
         <v>428</v>
       </c>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A216" s="3" t="s">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216" s="7" t="s">
         <v>429</v>
       </c>
       <c r="B216" s="3" t="s">
@@ -4278,8 +4284,8 @@
         <v>430</v>
       </c>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A217" s="3" t="s">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A217" s="7" t="s">
         <v>431</v>
       </c>
       <c r="B217" s="3" t="s">
@@ -4289,8 +4295,8 @@
         <v>432</v>
       </c>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A218" s="3" t="s">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A218" s="7" t="s">
         <v>433</v>
       </c>
       <c r="B218" s="3" t="s">
@@ -4300,8 +4306,8 @@
         <v>434</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A219" s="3" t="s">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A219" s="7" t="s">
         <v>435</v>
       </c>
       <c r="B219" s="3" t="s">
@@ -4311,8 +4317,8 @@
         <v>436</v>
       </c>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A220" s="3" t="s">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A220" s="7" t="s">
         <v>437</v>
       </c>
       <c r="B220" s="3" t="s">
@@ -4322,8 +4328,8 @@
         <v>438</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A221" s="3" t="s">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A221" s="7" t="s">
         <v>439</v>
       </c>
       <c r="B221" s="3" t="s">
@@ -4333,785 +4339,785 @@
         <v>440</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add smart chunking and improve NER prediction
Introduced a smart_chunk_text function for advanced text chunking based on list items, contact blocks, and hashtags. Refactored VietnameseNERPredictor to use this chunking for more robust NER predictions, including offset correction and entity grouping. Added syt-ner-traditional.ipynb for Kaggle-compatible NER training and processing. Updated .gitignore to exclude model directory.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1690,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="B223" sqref="B223"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>